<commit_message>
Lista 28/11 + update do BI
</commit_message>
<xml_diff>
--- a/DataBank/Fato.xlsx
+++ b/DataBank/Fato.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\PI3_2022\DataBank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FC5362-B7CC-4BD8-90F5-5D62C253EA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6A0DFE-43C5-461E-9E71-9B863FF4263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="394">
   <si>
     <t>ID</t>
   </si>
@@ -939,9 +939,6 @@
     <t>Horror,Comedia,Fantasia</t>
   </si>
   <si>
-    <t>Ação,8</t>
-  </si>
-  <si>
     <t>Suspense,Misterio</t>
   </si>
   <si>
@@ -1023,9 +1020,6 @@
     <t>Ação,Aventura,Misterio,Comedia,Crime</t>
   </si>
   <si>
-    <t>Suspense,8</t>
-  </si>
-  <si>
     <t>Ação,Aventura,Ficção Cientifica,Fantasia,Suspense</t>
   </si>
   <si>
@@ -1245,10 +1239,10 @@
     <t>Suspense,Terror,Crime</t>
   </si>
   <si>
-    <t>Terror.Ficção Cientifica</t>
-  </si>
-  <si>
     <t>Ficção Cientifica,Ação</t>
+  </si>
+  <si>
+    <t>Terror,Ficção Cientifica</t>
   </si>
 </sst>
 </file>
@@ -1309,7 +1303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1318,7 +1312,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1633,11 +1626,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1222"/>
+  <dimension ref="A1:H1241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1211" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1222" sqref="A1222"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9799,7 +9790,7 @@
         <v>117</v>
       </c>
       <c r="C559" t="s">
-        <v>292</v>
+        <v>190</v>
       </c>
       <c r="D559" s="6">
         <v>44855</v>
@@ -10051,7 +10042,7 @@
         <v>117</v>
       </c>
       <c r="C577" t="s">
-        <v>292</v>
+        <v>190</v>
       </c>
       <c r="D577" s="6">
         <v>44855</v>
@@ -10107,7 +10098,7 @@
         <v>46</v>
       </c>
       <c r="C581" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D581" s="6">
         <v>44827</v>
@@ -10289,7 +10280,7 @@
         <v>117</v>
       </c>
       <c r="C594" t="s">
-        <v>292</v>
+        <v>190</v>
       </c>
       <c r="D594" s="6">
         <v>44855</v>
@@ -10373,7 +10364,7 @@
         <v>46</v>
       </c>
       <c r="C600" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D600" s="6">
         <v>44827</v>
@@ -10429,7 +10420,7 @@
         <v>39</v>
       </c>
       <c r="C604" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D604" s="6">
         <v>44825</v>
@@ -10667,7 +10658,7 @@
         <v>117</v>
       </c>
       <c r="C621" t="s">
-        <v>292</v>
+        <v>190</v>
       </c>
       <c r="D621" s="6">
         <v>44855</v>
@@ -10681,7 +10672,7 @@
         <v>39</v>
       </c>
       <c r="C622" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D622" s="6">
         <v>44825</v>
@@ -10709,7 +10700,7 @@
         <v>123</v>
       </c>
       <c r="C624" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D624" s="6">
         <v>44853</v>
@@ -10793,7 +10784,7 @@
         <v>124</v>
       </c>
       <c r="C630" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D630" s="6">
         <v>44849</v>
@@ -10891,7 +10882,7 @@
         <v>126</v>
       </c>
       <c r="C637" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D637" s="6">
         <v>44972</v>
@@ -10975,7 +10966,7 @@
         <v>123</v>
       </c>
       <c r="C643" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D643" s="6">
         <v>44853</v>
@@ -10989,7 +10980,7 @@
         <v>39</v>
       </c>
       <c r="C644" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D644" s="6">
         <v>44825</v>
@@ -11059,7 +11050,7 @@
         <v>124</v>
       </c>
       <c r="C649" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D649" s="6">
         <v>44860</v>
@@ -11087,7 +11078,7 @@
         <v>127</v>
       </c>
       <c r="C651" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D651" s="6">
         <v>44861</v>
@@ -11255,7 +11246,7 @@
         <v>128</v>
       </c>
       <c r="C663" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D663" s="6">
         <v>44841</v>
@@ -11269,7 +11260,7 @@
         <v>123</v>
       </c>
       <c r="C664" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D664" s="6">
         <v>44853</v>
@@ -11283,7 +11274,7 @@
         <v>39</v>
       </c>
       <c r="C665" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D665" s="6">
         <v>44825</v>
@@ -11297,7 +11288,7 @@
         <v>91</v>
       </c>
       <c r="C666" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D666" s="6">
         <v>44853</v>
@@ -11339,7 +11330,7 @@
         <v>124</v>
       </c>
       <c r="C669" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D669" s="6">
         <v>44860</v>
@@ -11353,7 +11344,7 @@
         <v>129</v>
       </c>
       <c r="C670" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D670" s="6">
         <v>44855</v>
@@ -11367,7 +11358,7 @@
         <v>127</v>
       </c>
       <c r="C671" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D671" s="6">
         <v>44861</v>
@@ -11381,7 +11372,7 @@
         <v>130</v>
       </c>
       <c r="C672" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D672" s="6">
         <v>43857</v>
@@ -11423,7 +11414,7 @@
         <v>115</v>
       </c>
       <c r="C675" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D675" s="6">
         <v>44820</v>
@@ -11521,7 +11512,7 @@
         <v>128</v>
       </c>
       <c r="C682" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D682" s="6">
         <v>44841</v>
@@ -11549,7 +11540,7 @@
         <v>123</v>
       </c>
       <c r="C684" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D684" s="6">
         <v>44853</v>
@@ -11563,7 +11554,7 @@
         <v>130</v>
       </c>
       <c r="C685" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D685" s="6">
         <v>44862</v>
@@ -11577,7 +11568,7 @@
         <v>129</v>
       </c>
       <c r="C686" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D686" s="6">
         <v>44855</v>
@@ -11591,7 +11582,7 @@
         <v>39</v>
       </c>
       <c r="C687" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D687" s="6">
         <v>44825</v>
@@ -11633,7 +11624,7 @@
         <v>124</v>
       </c>
       <c r="C690" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D690" s="6">
         <v>44860</v>
@@ -11647,7 +11638,7 @@
         <v>127</v>
       </c>
       <c r="C691" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D691" s="6">
         <v>44861</v>
@@ -11703,7 +11694,7 @@
         <v>91</v>
       </c>
       <c r="C695" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D695" s="6">
         <v>44853</v>
@@ -11717,7 +11708,7 @@
         <v>134</v>
       </c>
       <c r="C696" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D696" s="6">
         <v>44798</v>
@@ -11815,7 +11806,7 @@
         <v>128</v>
       </c>
       <c r="C703" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D703" s="6">
         <v>44841</v>
@@ -11829,7 +11820,7 @@
         <v>123</v>
       </c>
       <c r="C704" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D704" s="6">
         <v>44853</v>
@@ -11843,7 +11834,7 @@
         <v>130</v>
       </c>
       <c r="C705" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D705" s="6">
         <v>44862</v>
@@ -11857,7 +11848,7 @@
         <v>91</v>
       </c>
       <c r="C706" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D706" s="6">
         <v>44853</v>
@@ -11871,7 +11862,7 @@
         <v>129</v>
       </c>
       <c r="C707" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D707" s="6">
         <v>44855</v>
@@ -11885,7 +11876,7 @@
         <v>39</v>
       </c>
       <c r="C708" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D708" s="6">
         <v>44825</v>
@@ -11941,7 +11932,7 @@
         <v>124</v>
       </c>
       <c r="C712" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D712" s="6">
         <v>44860</v>
@@ -11969,7 +11960,7 @@
         <v>134</v>
       </c>
       <c r="C714" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D714" s="6">
         <v>44798</v>
@@ -11983,7 +11974,7 @@
         <v>127</v>
       </c>
       <c r="C715" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D715" s="6">
         <v>44861</v>
@@ -12081,7 +12072,7 @@
         <v>128</v>
       </c>
       <c r="C722" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D722" s="6">
         <v>44841</v>
@@ -12109,7 +12100,7 @@
         <v>123</v>
       </c>
       <c r="C724" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D724" s="6">
         <v>44853</v>
@@ -12123,7 +12114,7 @@
         <v>129</v>
       </c>
       <c r="C725" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D725" s="6">
         <v>44855</v>
@@ -12137,7 +12128,7 @@
         <v>91</v>
       </c>
       <c r="C726" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D726" s="6">
         <v>44853</v>
@@ -12151,7 +12142,7 @@
         <v>39</v>
       </c>
       <c r="C727" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D727" s="6">
         <v>44825</v>
@@ -12193,7 +12184,7 @@
         <v>130</v>
       </c>
       <c r="C730" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D730" s="6">
         <v>44862</v>
@@ -12319,7 +12310,7 @@
         <v>127</v>
       </c>
       <c r="C739" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D739" s="6">
         <v>44861</v>
@@ -12347,7 +12338,7 @@
         <v>124</v>
       </c>
       <c r="C741" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D741" s="6">
         <v>44860</v>
@@ -12361,7 +12352,7 @@
         <v>128</v>
       </c>
       <c r="C742" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D742" s="6">
         <v>44841</v>
@@ -12375,7 +12366,7 @@
         <v>135</v>
       </c>
       <c r="C743" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D743" s="6">
         <v>44813</v>
@@ -12389,7 +12380,7 @@
         <v>136</v>
       </c>
       <c r="C744" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D744" s="6">
         <v>44866</v>
@@ -12417,7 +12408,7 @@
         <v>123</v>
       </c>
       <c r="C746" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D746" s="6">
         <v>44853</v>
@@ -12431,7 +12422,7 @@
         <v>129</v>
       </c>
       <c r="C747" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D747" s="6">
         <v>44855</v>
@@ -12487,7 +12478,7 @@
         <v>130</v>
       </c>
       <c r="C751" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D751" s="6">
         <v>44862</v>
@@ -12501,7 +12492,7 @@
         <v>39</v>
       </c>
       <c r="C752" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D752" s="6">
         <v>44825</v>
@@ -12529,7 +12520,7 @@
         <v>91</v>
       </c>
       <c r="C754" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D754" s="6">
         <v>44853</v>
@@ -12599,7 +12590,7 @@
         <v>137</v>
       </c>
       <c r="C759" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D759" s="6">
         <v>44819</v>
@@ -12641,7 +12632,7 @@
         <v>128</v>
       </c>
       <c r="C762" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D762" s="6">
         <v>44841</v>
@@ -12655,7 +12646,7 @@
         <v>135</v>
       </c>
       <c r="C763" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D763" s="6">
         <v>44813</v>
@@ -12669,7 +12660,7 @@
         <v>137</v>
       </c>
       <c r="C764" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D764" s="6">
         <v>44819</v>
@@ -12697,7 +12688,7 @@
         <v>138</v>
       </c>
       <c r="C766" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D766" s="6">
         <v>44866</v>
@@ -12711,7 +12702,7 @@
         <v>91</v>
       </c>
       <c r="C767" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D767" s="6">
         <v>44853</v>
@@ -12781,7 +12772,7 @@
         <v>129</v>
       </c>
       <c r="C772" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D772" s="6">
         <v>44855</v>
@@ -12795,7 +12786,7 @@
         <v>139</v>
       </c>
       <c r="C773" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D773" s="6">
         <v>44909</v>
@@ -12809,7 +12800,7 @@
         <v>123</v>
       </c>
       <c r="C774" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D774" s="6">
         <v>44853</v>
@@ -12851,7 +12842,7 @@
         <v>39</v>
       </c>
       <c r="C777" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D777" s="6">
         <v>44825</v>
@@ -12907,7 +12898,7 @@
         <v>140</v>
       </c>
       <c r="C781" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D781" s="6">
         <v>44701</v>
@@ -12921,7 +12912,7 @@
         <v>137</v>
       </c>
       <c r="C782" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D782" s="6">
         <v>44819</v>
@@ -12935,7 +12926,7 @@
         <v>135</v>
       </c>
       <c r="C783" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D783" s="6">
         <v>44813</v>
@@ -12949,7 +12940,7 @@
         <v>138</v>
       </c>
       <c r="C784" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D784" s="6">
         <v>44866</v>
@@ -12963,7 +12954,7 @@
         <v>128</v>
       </c>
       <c r="C785" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D785" s="6">
         <v>44841</v>
@@ -12991,7 +12982,7 @@
         <v>91</v>
       </c>
       <c r="C787" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D787" s="6">
         <v>44853</v>
@@ -13033,7 +13024,7 @@
         <v>139</v>
       </c>
       <c r="C790" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D790" s="6">
         <v>44909</v>
@@ -13061,7 +13052,7 @@
         <v>129</v>
       </c>
       <c r="C792" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D792" s="6">
         <v>44855</v>
@@ -13075,7 +13066,7 @@
         <v>123</v>
       </c>
       <c r="C793" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D793" s="6">
         <v>44853</v>
@@ -13131,7 +13122,7 @@
         <v>39</v>
       </c>
       <c r="C797" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D797" s="6">
         <v>44825</v>
@@ -13201,7 +13192,7 @@
         <v>142</v>
       </c>
       <c r="C802" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D802" s="6">
         <v>44869</v>
@@ -13215,7 +13206,7 @@
         <v>135</v>
       </c>
       <c r="C803" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D803" s="6">
         <v>44813</v>
@@ -13229,7 +13220,7 @@
         <v>137</v>
       </c>
       <c r="C804" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D804" s="6">
         <v>44819</v>
@@ -13271,7 +13262,7 @@
         <v>128</v>
       </c>
       <c r="C807" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D807" s="6">
         <v>44841</v>
@@ -13285,7 +13276,7 @@
         <v>138</v>
       </c>
       <c r="C808" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D808" s="6">
         <v>44866</v>
@@ -13341,7 +13332,7 @@
         <v>91</v>
       </c>
       <c r="C812" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D812" s="6">
         <v>44853</v>
@@ -13369,7 +13360,7 @@
         <v>146</v>
       </c>
       <c r="C814" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D814" s="6">
         <v>44812</v>
@@ -13383,7 +13374,7 @@
         <v>147</v>
       </c>
       <c r="C815" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D815" s="6">
         <v>44869</v>
@@ -13397,7 +13388,7 @@
         <v>139</v>
       </c>
       <c r="C816" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D816" s="6">
         <v>44909</v>
@@ -13467,7 +13458,7 @@
         <v>123</v>
       </c>
       <c r="C821" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D821" s="6">
         <v>44853</v>
@@ -13481,7 +13472,7 @@
         <v>142</v>
       </c>
       <c r="C822" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D822" s="6">
         <v>44869</v>
@@ -13523,7 +13514,7 @@
         <v>147</v>
       </c>
       <c r="C825" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D825" s="6">
         <v>44869</v>
@@ -13537,7 +13528,7 @@
         <v>135</v>
       </c>
       <c r="C826" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D826" s="6">
         <v>44813</v>
@@ -13551,7 +13542,7 @@
         <v>146</v>
       </c>
       <c r="C827" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D827" s="6">
         <v>44812</v>
@@ -13579,7 +13570,7 @@
         <v>137</v>
       </c>
       <c r="C829" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D829" s="6">
         <v>44819</v>
@@ -13607,7 +13598,7 @@
         <v>128</v>
       </c>
       <c r="C831" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D831" s="6">
         <v>44841</v>
@@ -13621,7 +13612,7 @@
         <v>138</v>
       </c>
       <c r="C832" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D832" s="6">
         <v>44866</v>
@@ -13635,7 +13626,7 @@
         <v>149</v>
       </c>
       <c r="C833" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D833" s="6">
         <v>44097</v>
@@ -13649,7 +13640,7 @@
         <v>91</v>
       </c>
       <c r="C834" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D834" s="6">
         <v>44853</v>
@@ -13691,7 +13682,7 @@
         <v>151</v>
       </c>
       <c r="C837" t="s">
-        <v>320</v>
+        <v>255</v>
       </c>
       <c r="D837" s="6">
         <v>44869</v>
@@ -13705,7 +13696,7 @@
         <v>71</v>
       </c>
       <c r="C838" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D838" s="6">
         <v>44874</v>
@@ -13761,7 +13752,7 @@
         <v>142</v>
       </c>
       <c r="C842" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D842" s="6">
         <v>44869</v>
@@ -13803,7 +13794,7 @@
         <v>135</v>
       </c>
       <c r="C845" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D845" s="6">
         <v>44813</v>
@@ -13817,7 +13808,7 @@
         <v>147</v>
       </c>
       <c r="C846" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D846" s="6">
         <v>44869</v>
@@ -13831,7 +13822,7 @@
         <v>146</v>
       </c>
       <c r="C847" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D847" s="6">
         <v>44812</v>
@@ -13859,7 +13850,7 @@
         <v>128</v>
       </c>
       <c r="C849" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D849" s="6">
         <v>44841</v>
@@ -13887,7 +13878,7 @@
         <v>137</v>
       </c>
       <c r="C851" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D851" s="6">
         <v>44819</v>
@@ -13901,7 +13892,7 @@
         <v>149</v>
       </c>
       <c r="C852" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D852" s="6">
         <v>44097</v>
@@ -13915,7 +13906,7 @@
         <v>151</v>
       </c>
       <c r="C853" t="s">
-        <v>320</v>
+        <v>255</v>
       </c>
       <c r="D853" s="6">
         <v>44869</v>
@@ -13943,7 +13934,7 @@
         <v>91</v>
       </c>
       <c r="C855" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D855" s="6">
         <v>44853</v>
@@ -13957,7 +13948,7 @@
         <v>71</v>
       </c>
       <c r="C856" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D856" s="6">
         <v>44874</v>
@@ -13985,7 +13976,7 @@
         <v>138</v>
       </c>
       <c r="C858" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D858" s="6">
         <v>44866</v>
@@ -14013,7 +14004,7 @@
         <v>152</v>
       </c>
       <c r="C860" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D860" s="6">
         <v>44880</v>
@@ -14041,7 +14032,7 @@
         <v>142</v>
       </c>
       <c r="C862" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D862" s="6">
         <v>44869</v>
@@ -14083,7 +14074,7 @@
         <v>147</v>
       </c>
       <c r="C865" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D865" s="6">
         <v>44869</v>
@@ -14097,7 +14088,7 @@
         <v>152</v>
       </c>
       <c r="C866" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D866" s="6">
         <v>44880</v>
@@ -14111,7 +14102,7 @@
         <v>128</v>
       </c>
       <c r="C867" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D867" s="6">
         <v>44841</v>
@@ -14125,7 +14116,7 @@
         <v>146</v>
       </c>
       <c r="C868" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D868" s="6">
         <v>44812</v>
@@ -14153,7 +14144,7 @@
         <v>135</v>
       </c>
       <c r="C870" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D870" s="6">
         <v>44813</v>
@@ -14195,7 +14186,7 @@
         <v>91</v>
       </c>
       <c r="C873" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D873" s="6">
         <v>44853</v>
@@ -14223,7 +14214,7 @@
         <v>137</v>
       </c>
       <c r="C875" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D875" s="6">
         <v>44819</v>
@@ -14237,7 +14228,7 @@
         <v>149</v>
       </c>
       <c r="C876" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D876" s="6">
         <v>44097</v>
@@ -14279,7 +14270,7 @@
         <v>151</v>
       </c>
       <c r="C879" t="s">
-        <v>320</v>
+        <v>255</v>
       </c>
       <c r="D879" s="6">
         <v>44869</v>
@@ -14307,7 +14298,7 @@
         <v>138</v>
       </c>
       <c r="C881" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D881" s="6">
         <v>44866</v>
@@ -14321,7 +14312,7 @@
         <v>142</v>
       </c>
       <c r="C882" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D882" s="6">
         <v>44869</v>
@@ -14349,7 +14340,7 @@
         <v>152</v>
       </c>
       <c r="C884" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D884" s="6">
         <v>44880</v>
@@ -14391,7 +14382,7 @@
         <v>128</v>
       </c>
       <c r="C887" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D887" s="6">
         <v>44841</v>
@@ -14405,7 +14396,7 @@
         <v>135</v>
       </c>
       <c r="C888" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D888" s="6">
         <v>44813</v>
@@ -14419,7 +14410,7 @@
         <v>146</v>
       </c>
       <c r="C889" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D889" s="6">
         <v>44812</v>
@@ -14433,7 +14424,7 @@
         <v>147</v>
       </c>
       <c r="C890" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D890" s="6">
         <v>44869</v>
@@ -14447,7 +14438,7 @@
         <v>91</v>
       </c>
       <c r="C891" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D891" s="6">
         <v>44853</v>
@@ -14503,7 +14494,7 @@
         <v>137</v>
       </c>
       <c r="C895" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D895" s="6">
         <v>44819</v>
@@ -14517,7 +14508,7 @@
         <v>149</v>
       </c>
       <c r="C896" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D896" s="6">
         <v>44097</v>
@@ -14531,7 +14522,7 @@
         <v>93</v>
       </c>
       <c r="C897" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D897" s="6">
         <v>44812</v>
@@ -14601,7 +14592,7 @@
         <v>142</v>
       </c>
       <c r="C902" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D902" s="6">
         <v>44869</v>
@@ -14629,7 +14620,7 @@
         <v>152</v>
       </c>
       <c r="C904" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D904" s="6">
         <v>44880</v>
@@ -14643,7 +14634,7 @@
         <v>93</v>
       </c>
       <c r="C905" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D905" s="6">
         <v>44812</v>
@@ -14671,7 +14662,7 @@
         <v>128</v>
       </c>
       <c r="C907" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D907" s="6">
         <v>44841</v>
@@ -14699,7 +14690,7 @@
         <v>153</v>
       </c>
       <c r="C909" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D909" s="6">
         <v>44874</v>
@@ -14713,7 +14704,7 @@
         <v>91</v>
       </c>
       <c r="C910" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D910" s="6">
         <v>44853</v>
@@ -14741,7 +14732,7 @@
         <v>146</v>
       </c>
       <c r="C912" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D912" s="6">
         <v>44812</v>
@@ -14755,7 +14746,7 @@
         <v>147</v>
       </c>
       <c r="C913" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D913" s="6">
         <v>44869</v>
@@ -14769,7 +14760,7 @@
         <v>135</v>
       </c>
       <c r="C914" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D914" s="6">
         <v>44813</v>
@@ -14825,7 +14816,7 @@
         <v>154</v>
       </c>
       <c r="C918" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D918" s="6">
         <v>44537</v>
@@ -14839,7 +14830,7 @@
         <v>137</v>
       </c>
       <c r="C919" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D919" s="6">
         <v>44819</v>
@@ -14853,7 +14844,7 @@
         <v>155</v>
       </c>
       <c r="C920" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D920" s="6">
         <v>44868</v>
@@ -14895,7 +14886,7 @@
         <v>153</v>
       </c>
       <c r="C923" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D923" s="6">
         <v>44874</v>
@@ -14923,7 +14914,7 @@
         <v>152</v>
       </c>
       <c r="C925" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D925" s="6">
         <v>44880</v>
@@ -14937,7 +14928,7 @@
         <v>93</v>
       </c>
       <c r="C926" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D926" s="6">
         <v>44812</v>
@@ -14951,7 +14942,7 @@
         <v>157</v>
       </c>
       <c r="C927" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D927" s="6">
         <v>44875</v>
@@ -14965,7 +14956,7 @@
         <v>128</v>
       </c>
       <c r="C928" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D928" s="6">
         <v>44841</v>
@@ -14979,7 +14970,7 @@
         <v>158</v>
       </c>
       <c r="C929" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D929" s="6">
         <v>44797</v>
@@ -15007,7 +14998,7 @@
         <v>142</v>
       </c>
       <c r="C931" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D931" s="6">
         <v>44869</v>
@@ -15035,7 +15026,7 @@
         <v>147</v>
       </c>
       <c r="C933" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D933" s="6">
         <v>44869</v>
@@ -15049,7 +15040,7 @@
         <v>91</v>
       </c>
       <c r="C934" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D934" s="6">
         <v>44853</v>
@@ -15063,7 +15054,7 @@
         <v>146</v>
       </c>
       <c r="C935" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D935" s="6">
         <v>44812</v>
@@ -15091,7 +15082,7 @@
         <v>135</v>
       </c>
       <c r="C937" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D937" s="6">
         <v>44813</v>
@@ -15105,7 +15096,7 @@
         <v>155</v>
       </c>
       <c r="C938" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D938" s="6">
         <v>44868</v>
@@ -15133,7 +15124,7 @@
         <v>154</v>
       </c>
       <c r="C940" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D940" s="6">
         <v>44537</v>
@@ -15175,7 +15166,7 @@
         <v>157</v>
       </c>
       <c r="C943" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D943" s="6">
         <v>44875</v>
@@ -15189,7 +15180,7 @@
         <v>159</v>
       </c>
       <c r="C944" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D944" s="6">
         <v>44831</v>
@@ -15203,7 +15194,7 @@
         <v>142</v>
       </c>
       <c r="C945" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D945" s="6">
         <v>44869</v>
@@ -15231,7 +15222,7 @@
         <v>153</v>
       </c>
       <c r="C947" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D947" s="6">
         <v>44874</v>
@@ -15245,7 +15236,7 @@
         <v>158</v>
       </c>
       <c r="C948" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D948" s="6">
         <v>44797</v>
@@ -15273,7 +15264,7 @@
         <v>161</v>
       </c>
       <c r="C950" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D950" s="6">
         <v>44869</v>
@@ -15287,7 +15278,7 @@
         <v>152</v>
       </c>
       <c r="C951" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D951" s="6">
         <v>44880</v>
@@ -15301,7 +15292,7 @@
         <v>93</v>
       </c>
       <c r="C952" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D952" s="6">
         <v>44812</v>
@@ -15315,7 +15306,7 @@
         <v>128</v>
       </c>
       <c r="C953" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D953" s="6">
         <v>44841</v>
@@ -15329,7 +15320,7 @@
         <v>91</v>
       </c>
       <c r="C954" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D954" s="6">
         <v>44853</v>
@@ -15385,7 +15376,7 @@
         <v>162</v>
       </c>
       <c r="C958" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D958" s="6">
         <v>44876</v>
@@ -15399,7 +15390,7 @@
         <v>163</v>
       </c>
       <c r="C959" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D959" s="6">
         <v>44666</v>
@@ -15427,7 +15418,7 @@
         <v>164</v>
       </c>
       <c r="C961" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D961" s="6">
         <v>44001</v>
@@ -15455,7 +15446,7 @@
         <v>159</v>
       </c>
       <c r="C963" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D963" s="6">
         <v>44831</v>
@@ -15469,7 +15460,7 @@
         <v>157</v>
       </c>
       <c r="C964" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D964" s="6">
         <v>44875</v>
@@ -15483,7 +15474,7 @@
         <v>161</v>
       </c>
       <c r="C965" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D965" s="6">
         <v>44869</v>
@@ -15497,7 +15488,7 @@
         <v>142</v>
       </c>
       <c r="C966" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D966" s="6">
         <v>44869</v>
@@ -15525,7 +15516,7 @@
         <v>158</v>
       </c>
       <c r="C968" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D968" s="6">
         <v>44797</v>
@@ -15539,7 +15530,7 @@
         <v>91</v>
       </c>
       <c r="C969" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D969" s="6">
         <v>44853</v>
@@ -15553,7 +15544,7 @@
         <v>153</v>
       </c>
       <c r="C970" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D970" s="6">
         <v>44874</v>
@@ -15581,7 +15572,7 @@
         <v>162</v>
       </c>
       <c r="C972" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D972" s="6">
         <v>44876</v>
@@ -15595,7 +15586,7 @@
         <v>152</v>
       </c>
       <c r="C973" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D973" s="6">
         <v>44880</v>
@@ -15609,7 +15600,7 @@
         <v>128</v>
       </c>
       <c r="C974" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D974" s="6">
         <v>44841</v>
@@ -15623,7 +15614,7 @@
         <v>165</v>
       </c>
       <c r="C975" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D975" s="6">
         <v>44876</v>
@@ -15651,7 +15642,7 @@
         <v>93</v>
       </c>
       <c r="C977" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D977" s="6">
         <v>44812</v>
@@ -15693,7 +15684,7 @@
         <v>163</v>
       </c>
       <c r="C980" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D980" s="6">
         <v>44666</v>
@@ -15735,7 +15726,7 @@
         <v>159</v>
       </c>
       <c r="C983" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D983" s="6">
         <v>44831</v>
@@ -15749,7 +15740,7 @@
         <v>157</v>
       </c>
       <c r="C984" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D984" s="6">
         <v>44875</v>
@@ -15777,7 +15768,7 @@
         <v>161</v>
       </c>
       <c r="C986" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D986" s="6">
         <v>44869</v>
@@ -15805,7 +15796,7 @@
         <v>91</v>
       </c>
       <c r="C988" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D988" s="6">
         <v>44853</v>
@@ -15819,7 +15810,7 @@
         <v>142</v>
       </c>
       <c r="C989" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D989" s="6">
         <v>44869</v>
@@ -15833,7 +15824,7 @@
         <v>153</v>
       </c>
       <c r="C990" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D990" s="6">
         <v>44874</v>
@@ -15861,7 +15852,7 @@
         <v>165</v>
       </c>
       <c r="C992" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D992" s="6">
         <v>44876</v>
@@ -15875,7 +15866,7 @@
         <v>162</v>
       </c>
       <c r="C993" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D993" s="6">
         <v>44876</v>
@@ -15917,7 +15908,7 @@
         <v>152</v>
       </c>
       <c r="C996" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D996" s="6">
         <v>44880</v>
@@ -15931,7 +15922,7 @@
         <v>158</v>
       </c>
       <c r="C997" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D997" s="6">
         <v>44797</v>
@@ -15959,7 +15950,7 @@
         <v>128</v>
       </c>
       <c r="C999" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D999" s="6">
         <v>44841</v>
@@ -15973,7 +15964,7 @@
         <v>93</v>
       </c>
       <c r="C1000" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D1000" s="6">
         <v>44812</v>
@@ -16015,7 +16006,7 @@
         <v>159</v>
       </c>
       <c r="C1003" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D1003" s="6">
         <v>44831</v>
@@ -16043,7 +16034,7 @@
         <v>161</v>
       </c>
       <c r="C1005" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D1005" s="6">
         <v>44869</v>
@@ -16057,7 +16048,7 @@
         <v>157</v>
       </c>
       <c r="C1006" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D1006" s="6">
         <v>44875</v>
@@ -16085,7 +16076,7 @@
         <v>142</v>
       </c>
       <c r="C1008" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D1008" s="6">
         <v>44869</v>
@@ -16099,7 +16090,7 @@
         <v>165</v>
       </c>
       <c r="C1009" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D1009" s="6">
         <v>44876</v>
@@ -16113,7 +16104,7 @@
         <v>91</v>
       </c>
       <c r="C1010" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1010" s="6">
         <v>44853</v>
@@ -16127,7 +16118,7 @@
         <v>162</v>
       </c>
       <c r="C1011" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D1011" s="6">
         <v>44876</v>
@@ -16141,7 +16132,7 @@
         <v>158</v>
       </c>
       <c r="C1012" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D1012" s="6">
         <v>44797</v>
@@ -16155,7 +16146,7 @@
         <v>152</v>
       </c>
       <c r="C1013" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D1013" s="6">
         <v>44880</v>
@@ -16211,7 +16202,7 @@
         <v>153</v>
       </c>
       <c r="C1017" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D1017" s="6">
         <v>44874</v>
@@ -16253,7 +16244,7 @@
         <v>128</v>
       </c>
       <c r="C1020" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D1020" s="6">
         <v>44841</v>
@@ -16267,7 +16258,7 @@
         <v>39</v>
       </c>
       <c r="C1021" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D1021" s="6">
         <v>44825</v>
@@ -16309,7 +16300,7 @@
         <v>159</v>
       </c>
       <c r="C1024" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D1024" s="6">
         <v>44831</v>
@@ -16323,7 +16314,7 @@
         <v>168</v>
       </c>
       <c r="C1025" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D1025" s="6">
         <v>44841</v>
@@ -16351,7 +16342,7 @@
         <v>157</v>
       </c>
       <c r="C1027" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D1027" s="6">
         <v>44875</v>
@@ -16365,7 +16356,7 @@
         <v>161</v>
       </c>
       <c r="C1028" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D1028" s="6">
         <v>44869</v>
@@ -16393,7 +16384,7 @@
         <v>165</v>
       </c>
       <c r="C1030" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D1030" s="6">
         <v>44876</v>
@@ -16407,7 +16398,7 @@
         <v>142</v>
       </c>
       <c r="C1031" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D1031" s="6">
         <v>44869</v>
@@ -16421,7 +16412,7 @@
         <v>152</v>
       </c>
       <c r="C1032" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D1032" s="6">
         <v>44880</v>
@@ -16449,7 +16440,7 @@
         <v>91</v>
       </c>
       <c r="C1034" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1034" s="6">
         <v>44853</v>
@@ -16477,7 +16468,7 @@
         <v>169</v>
       </c>
       <c r="C1036" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D1036" s="6">
         <v>44876</v>
@@ -16505,7 +16496,7 @@
         <v>162</v>
       </c>
       <c r="C1038" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D1038" s="6">
         <v>44876</v>
@@ -16533,7 +16524,7 @@
         <v>158</v>
       </c>
       <c r="C1040" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D1040" s="6">
         <v>44797</v>
@@ -16547,7 +16538,7 @@
         <v>170</v>
       </c>
       <c r="C1041" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D1041" s="6">
         <v>44848</v>
@@ -16589,7 +16580,7 @@
         <v>91</v>
       </c>
       <c r="C1044" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1044" s="6">
         <v>44853</v>
@@ -16617,7 +16608,7 @@
         <v>168</v>
       </c>
       <c r="C1046" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D1046" s="6">
         <v>44841</v>
@@ -16645,7 +16636,7 @@
         <v>172</v>
       </c>
       <c r="C1048" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D1048" s="6">
         <v>44880</v>
@@ -16659,7 +16650,7 @@
         <v>157</v>
       </c>
       <c r="C1049" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D1049" s="6">
         <v>44875</v>
@@ -16673,7 +16664,7 @@
         <v>142</v>
       </c>
       <c r="C1050" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D1050" s="6">
         <v>44869</v>
@@ -16687,7 +16678,7 @@
         <v>159</v>
       </c>
       <c r="C1051" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D1051" s="6">
         <v>44831</v>
@@ -16701,7 +16692,7 @@
         <v>161</v>
       </c>
       <c r="C1052" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D1052" s="6">
         <v>44869</v>
@@ -16715,7 +16706,7 @@
         <v>152</v>
       </c>
       <c r="C1053" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D1053" s="6">
         <v>44880</v>
@@ -16743,7 +16734,7 @@
         <v>170</v>
       </c>
       <c r="C1055" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D1055" s="6">
         <v>44848</v>
@@ -16757,7 +16748,7 @@
         <v>165</v>
       </c>
       <c r="C1056" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D1056" s="6">
         <v>44876</v>
@@ -16785,7 +16776,7 @@
         <v>128</v>
       </c>
       <c r="C1058" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D1058" s="6">
         <v>44841</v>
@@ -16841,7 +16832,7 @@
         <v>91</v>
       </c>
       <c r="C1062" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1062" s="6">
         <v>44853</v>
@@ -16869,7 +16860,7 @@
         <v>171</v>
       </c>
       <c r="C1064" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D1064" s="6">
         <v>44867</v>
@@ -16883,7 +16874,7 @@
         <v>168</v>
       </c>
       <c r="C1065" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D1065" s="6">
         <v>44841</v>
@@ -16897,7 +16888,7 @@
         <v>60</v>
       </c>
       <c r="C1066" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D1066" s="6">
         <v>44827</v>
@@ -16925,7 +16916,7 @@
         <v>159</v>
       </c>
       <c r="C1068" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D1068" s="6">
         <v>44831</v>
@@ -16939,7 +16930,7 @@
         <v>172</v>
       </c>
       <c r="C1069" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D1069" s="6">
         <v>44880</v>
@@ -16953,7 +16944,7 @@
         <v>174</v>
       </c>
       <c r="C1070" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D1070" s="6">
         <v>44589</v>
@@ -16995,7 +16986,7 @@
         <v>167</v>
       </c>
       <c r="C1073" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D1073" s="6">
         <v>44881</v>
@@ -17009,7 +17000,7 @@
         <v>176</v>
       </c>
       <c r="C1074" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D1074" s="6">
         <v>44903</v>
@@ -17023,7 +17014,7 @@
         <v>170</v>
       </c>
       <c r="C1075" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D1075" s="6">
         <v>44848</v>
@@ -17037,7 +17028,7 @@
         <v>152</v>
       </c>
       <c r="C1076" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D1076" s="6">
         <v>44880</v>
@@ -17065,7 +17056,7 @@
         <v>157</v>
       </c>
       <c r="C1078" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D1078" s="6">
         <v>44875</v>
@@ -17093,7 +17084,7 @@
         <v>142</v>
       </c>
       <c r="C1080" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D1080" s="6">
         <v>44869</v>
@@ -17135,7 +17126,7 @@
         <v>171</v>
       </c>
       <c r="C1083" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D1083" s="6">
         <v>44867</v>
@@ -17149,7 +17140,7 @@
         <v>91</v>
       </c>
       <c r="C1084" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1084" s="6">
         <v>44853</v>
@@ -17163,7 +17154,7 @@
         <v>60</v>
       </c>
       <c r="C1085" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D1085" s="6">
         <v>44827</v>
@@ -17191,7 +17182,7 @@
         <v>168</v>
       </c>
       <c r="C1087" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D1087" s="6">
         <v>44841</v>
@@ -17219,7 +17210,7 @@
         <v>159</v>
       </c>
       <c r="C1089" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D1089" s="6">
         <v>44831</v>
@@ -17233,7 +17224,7 @@
         <v>176</v>
       </c>
       <c r="C1090" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D1090" s="6">
         <v>44903</v>
@@ -17247,7 +17238,7 @@
         <v>172</v>
       </c>
       <c r="C1091" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D1091" s="6">
         <v>44880</v>
@@ -17261,7 +17252,7 @@
         <v>180</v>
       </c>
       <c r="C1092" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D1092" s="6">
         <v>44883</v>
@@ -17275,7 +17266,7 @@
         <v>174</v>
       </c>
       <c r="C1093" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D1093" s="6">
         <v>44589</v>
@@ -17289,7 +17280,7 @@
         <v>181</v>
       </c>
       <c r="C1094" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D1094" s="6">
         <v>44883</v>
@@ -17303,7 +17294,7 @@
         <v>167</v>
       </c>
       <c r="C1095" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D1095" s="6">
         <v>44881</v>
@@ -17359,7 +17350,7 @@
         <v>152</v>
       </c>
       <c r="C1099" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D1099" s="6">
         <v>44880</v>
@@ -17373,7 +17364,7 @@
         <v>157</v>
       </c>
       <c r="C1100" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D1100" s="6">
         <v>44875</v>
@@ -17401,7 +17392,7 @@
         <v>181</v>
       </c>
       <c r="C1102" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D1102" s="6">
         <v>44883</v>
@@ -17415,7 +17406,7 @@
         <v>180</v>
       </c>
       <c r="C1103" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D1103" s="6">
         <v>44874</v>
@@ -17443,7 +17434,7 @@
         <v>91</v>
       </c>
       <c r="C1105" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1105" s="6">
         <v>44853</v>
@@ -17485,7 +17476,7 @@
         <v>60</v>
       </c>
       <c r="C1108" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D1108" s="6">
         <v>44827</v>
@@ -17510,7 +17501,7 @@
         <v>457232</v>
       </c>
       <c r="B1110" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C1110" t="s">
         <v>193</v>
@@ -17527,7 +17518,7 @@
         <v>176</v>
       </c>
       <c r="C1111" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D1111" s="6">
         <v>44903</v>
@@ -17552,10 +17543,10 @@
         <v>754452</v>
       </c>
       <c r="B1113" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C1113" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D1113" s="6">
         <v>44883</v>
@@ -17569,7 +17560,7 @@
         <v>168</v>
       </c>
       <c r="C1114" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D1114" s="6">
         <v>44841</v>
@@ -17580,10 +17571,10 @@
         <v>939210</v>
       </c>
       <c r="B1115" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C1115" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D1115" s="6">
         <v>44883</v>
@@ -17597,7 +17588,7 @@
         <v>39</v>
       </c>
       <c r="C1116" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D1116" s="6">
         <v>44825</v>
@@ -17611,7 +17602,7 @@
         <v>159</v>
       </c>
       <c r="C1117" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D1117" s="6">
         <v>44831</v>
@@ -17625,7 +17616,7 @@
         <v>142</v>
       </c>
       <c r="C1118" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D1118" s="6">
         <v>44869</v>
@@ -17639,7 +17630,7 @@
         <v>172</v>
       </c>
       <c r="C1119" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D1119" s="6">
         <v>44810</v>
@@ -17664,10 +17655,10 @@
         <v>593643</v>
       </c>
       <c r="B1121" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C1121" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D1121" s="6">
         <v>44882</v>
@@ -17681,7 +17672,7 @@
         <v>181</v>
       </c>
       <c r="C1122" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D1122" s="6">
         <v>44883</v>
@@ -17695,7 +17686,7 @@
         <v>180</v>
       </c>
       <c r="C1123" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D1123" s="6">
         <v>44874</v>
@@ -17723,7 +17714,7 @@
         <v>91</v>
       </c>
       <c r="C1125" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1125" s="6">
         <v>44853</v>
@@ -17776,7 +17767,7 @@
         <v>457232</v>
       </c>
       <c r="B1129" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C1129" t="s">
         <v>193</v>
@@ -17793,7 +17784,7 @@
         <v>60</v>
       </c>
       <c r="C1130" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D1130" s="6">
         <v>44827</v>
@@ -17835,7 +17826,7 @@
         <v>176</v>
       </c>
       <c r="C1133" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D1133" s="6">
         <v>44903</v>
@@ -17849,7 +17840,7 @@
         <v>39</v>
       </c>
       <c r="C1134" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D1134" s="6">
         <v>44825</v>
@@ -17860,10 +17851,10 @@
         <v>754452</v>
       </c>
       <c r="B1135" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C1135" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D1135" s="6">
         <v>44883</v>
@@ -17874,10 +17865,10 @@
         <v>593643</v>
       </c>
       <c r="B1136" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C1136" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D1136" s="6">
         <v>44882</v>
@@ -17888,10 +17879,10 @@
         <v>939210</v>
       </c>
       <c r="B1137" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C1137" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D1137" s="6">
         <v>44883</v>
@@ -17905,7 +17896,7 @@
         <v>142</v>
       </c>
       <c r="C1138" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D1138" s="6">
         <v>44869</v>
@@ -17919,7 +17910,7 @@
         <v>168</v>
       </c>
       <c r="C1139" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D1139" s="6">
         <v>44841</v>
@@ -17961,7 +17952,7 @@
         <v>91</v>
       </c>
       <c r="C1142" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1142" s="6">
         <v>44853</v>
@@ -17975,7 +17966,7 @@
         <v>137</v>
       </c>
       <c r="C1143" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D1143" s="6">
         <v>44819</v>
@@ -17989,7 +17980,7 @@
         <v>181</v>
       </c>
       <c r="C1144" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D1144" s="6">
         <v>44881</v>
@@ -18000,10 +17991,10 @@
         <v>830784</v>
       </c>
       <c r="B1145" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C1145" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D1145" s="6">
         <v>44841</v>
@@ -18017,7 +18008,7 @@
         <v>180</v>
       </c>
       <c r="C1146" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D1146" s="6">
         <v>44874</v>
@@ -18042,7 +18033,7 @@
         <v>497828</v>
       </c>
       <c r="B1148" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C1148" t="s">
         <v>207</v>
@@ -18070,7 +18061,7 @@
         <v>615952</v>
       </c>
       <c r="B1150" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C1150" t="s">
         <v>193</v>
@@ -18087,7 +18078,7 @@
         <v>139</v>
       </c>
       <c r="C1151" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1151" s="6">
         <v>44909</v>
@@ -18098,7 +18089,7 @@
         <v>1049233</v>
       </c>
       <c r="B1152" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C1152" t="s">
         <v>198</v>
@@ -18112,7 +18103,7 @@
         <v>854239</v>
       </c>
       <c r="B1153" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C1153" t="s">
         <v>193</v>
@@ -18154,7 +18145,7 @@
         <v>821881</v>
       </c>
       <c r="B1156" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C1156" t="s">
         <v>289</v>
@@ -18171,7 +18162,7 @@
         <v>60</v>
       </c>
       <c r="C1157" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D1157" s="6">
         <v>44827</v>
@@ -18182,7 +18173,7 @@
         <v>457232</v>
       </c>
       <c r="B1158" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C1158" t="s">
         <v>193</v>
@@ -18196,10 +18187,10 @@
         <v>1038627</v>
       </c>
       <c r="B1159" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C1159" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D1159" s="6">
         <v>44888</v>
@@ -18210,10 +18201,10 @@
         <v>877269</v>
       </c>
       <c r="B1160" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C1160" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D1160" s="6">
         <v>44888</v>
@@ -18224,10 +18215,10 @@
         <v>593643</v>
       </c>
       <c r="B1161" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C1161" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D1161" s="6">
         <v>44882</v>
@@ -18241,7 +18232,7 @@
         <v>91</v>
       </c>
       <c r="C1162" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1162" s="6">
         <v>44853</v>
@@ -18252,10 +18243,10 @@
         <v>830784</v>
       </c>
       <c r="B1163" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C1163" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D1163" s="6">
         <v>44841</v>
@@ -18269,7 +18260,7 @@
         <v>137</v>
       </c>
       <c r="C1164" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D1164" s="6">
         <v>44819</v>
@@ -18280,7 +18271,7 @@
         <v>615952</v>
       </c>
       <c r="B1165" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C1165" t="s">
         <v>193</v>
@@ -18294,7 +18285,7 @@
         <v>1049233</v>
       </c>
       <c r="B1166" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C1166" t="s">
         <v>198</v>
@@ -18308,7 +18299,7 @@
         <v>821881</v>
       </c>
       <c r="B1167" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C1167" t="s">
         <v>289</v>
@@ -18339,7 +18330,7 @@
         <v>181</v>
       </c>
       <c r="C1169" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D1169" s="6">
         <v>44881</v>
@@ -18350,10 +18341,10 @@
         <v>1038627</v>
       </c>
       <c r="B1170" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C1170" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D1170" s="6">
         <v>44889</v>
@@ -18364,10 +18355,10 @@
         <v>736918</v>
       </c>
       <c r="B1171" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C1171" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D1171" s="6">
         <v>44889</v>
@@ -18381,7 +18372,7 @@
         <v>180</v>
       </c>
       <c r="C1172" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D1172" s="6">
         <v>44874</v>
@@ -18406,7 +18397,7 @@
         <v>497828</v>
       </c>
       <c r="B1174" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C1174" t="s">
         <v>207</v>
@@ -18420,7 +18411,7 @@
         <v>854239</v>
       </c>
       <c r="B1175" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C1175" t="s">
         <v>193</v>
@@ -18434,7 +18425,7 @@
         <v>1044043</v>
       </c>
       <c r="B1176" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C1176" t="s">
         <v>207</v>
@@ -18451,7 +18442,7 @@
         <v>139</v>
       </c>
       <c r="C1177" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1177" s="6">
         <v>44909</v>
@@ -18476,10 +18467,10 @@
         <v>877269</v>
       </c>
       <c r="B1179" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C1179" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D1179" s="6">
         <v>44888</v>
@@ -18507,7 +18498,7 @@
         <v>60</v>
       </c>
       <c r="C1181" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D1181" s="6">
         <v>44827</v>
@@ -18518,10 +18509,10 @@
         <v>774752</v>
       </c>
       <c r="B1182" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C1182" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D1182" s="6">
         <v>44890</v>
@@ -18535,7 +18526,7 @@
         <v>91</v>
       </c>
       <c r="C1183" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1183" s="6">
         <v>44853</v>
@@ -18546,10 +18537,10 @@
         <v>830784</v>
       </c>
       <c r="B1184" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C1184" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D1184" s="6">
         <v>44841</v>
@@ -18563,7 +18554,7 @@
         <v>137</v>
       </c>
       <c r="C1185" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D1185" s="6">
         <v>44819</v>
@@ -18574,7 +18565,7 @@
         <v>1049233</v>
       </c>
       <c r="B1186" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C1186" t="s">
         <v>198</v>
@@ -18588,10 +18579,10 @@
         <v>736918</v>
       </c>
       <c r="B1187" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C1187" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D1187" s="6">
         <v>44889</v>
@@ -18619,7 +18610,7 @@
         <v>181</v>
       </c>
       <c r="C1189" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D1189" s="6">
         <v>44881</v>
@@ -18633,7 +18624,7 @@
         <v>40</v>
       </c>
       <c r="C1190" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D1190" s="6">
         <v>44825</v>
@@ -18644,10 +18635,10 @@
         <v>1006917</v>
       </c>
       <c r="B1191" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C1191" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D1191" s="6">
         <v>44855</v>
@@ -18675,7 +18666,7 @@
         <v>180</v>
       </c>
       <c r="C1193" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D1193" s="6">
         <v>44874</v>
@@ -18686,7 +18677,7 @@
         <v>615952</v>
       </c>
       <c r="B1194" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C1194" t="s">
         <v>193</v>
@@ -18700,10 +18691,10 @@
         <v>1038627</v>
       </c>
       <c r="B1195" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C1195" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D1195" s="6">
         <v>44889</v>
@@ -18714,10 +18705,10 @@
         <v>987919</v>
       </c>
       <c r="B1196" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C1196" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D1196" s="6">
         <v>44889</v>
@@ -18728,7 +18719,7 @@
         <v>497828</v>
       </c>
       <c r="B1197" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C1197" t="s">
         <v>207</v>
@@ -18745,7 +18736,7 @@
         <v>139</v>
       </c>
       <c r="C1198" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D1198" s="6">
         <v>44909</v>
@@ -18756,10 +18747,10 @@
         <v>987919</v>
       </c>
       <c r="B1199" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C1199" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D1199" s="6">
         <v>44889</v>
@@ -18770,7 +18761,7 @@
         <v>821881</v>
       </c>
       <c r="B1200" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C1200" t="s">
         <v>289</v>
@@ -18784,7 +18775,7 @@
         <v>497828</v>
       </c>
       <c r="B1201" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C1201" t="s">
         <v>207</v>
@@ -18801,7 +18792,7 @@
         <v>91</v>
       </c>
       <c r="C1202" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D1202" s="6">
         <v>44853</v>
@@ -18815,7 +18806,7 @@
         <v>152</v>
       </c>
       <c r="C1203" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D1203" s="6">
         <v>44880</v>
@@ -18829,7 +18820,7 @@
         <v>181</v>
       </c>
       <c r="C1204" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D1204" s="6">
         <v>44881</v>
@@ -18840,10 +18831,10 @@
         <v>988233</v>
       </c>
       <c r="B1205" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C1205" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D1205" s="6">
         <v>44866</v>
@@ -18857,7 +18848,7 @@
         <v>165</v>
       </c>
       <c r="C1206" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D1206" s="6">
         <v>44876</v>
@@ -18885,7 +18876,7 @@
         <v>60</v>
       </c>
       <c r="C1208" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D1208" s="6">
         <v>44827</v>
@@ -18899,7 +18890,7 @@
         <v>93</v>
       </c>
       <c r="C1209" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D1209" s="6">
         <v>44812</v>
@@ -18924,10 +18915,10 @@
         <v>966220</v>
       </c>
       <c r="B1211" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C1211" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D1211" s="6">
         <v>44684</v>
@@ -18941,7 +18932,7 @@
         <v>157</v>
       </c>
       <c r="C1212" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D1212" s="6">
         <v>44875</v>
@@ -18952,10 +18943,10 @@
         <v>899294</v>
       </c>
       <c r="B1213" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C1213" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D1213" s="6">
         <v>44715</v>
@@ -18966,10 +18957,10 @@
         <v>846778</v>
       </c>
       <c r="B1214" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C1214" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D1214" s="6">
         <v>44813</v>
@@ -18983,7 +18974,7 @@
         <v>142</v>
       </c>
       <c r="C1215" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D1215" s="6">
         <v>44869</v>
@@ -19011,7 +19002,7 @@
         <v>158</v>
       </c>
       <c r="C1217" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D1217" s="6">
         <v>44797</v>
@@ -19025,7 +19016,7 @@
         <v>153</v>
       </c>
       <c r="C1218" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D1218" s="6">
         <v>44874</v>
@@ -19036,10 +19027,10 @@
         <v>872177</v>
       </c>
       <c r="B1219" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C1219" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D1219" s="6">
         <v>44680</v>
@@ -19067,14 +19058,291 @@
         <v>172</v>
       </c>
       <c r="C1221" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D1221" s="6">
         <v>44810</v>
       </c>
     </row>
     <row r="1222" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1222" s="8"/>
+      <c r="A1222">
+        <v>436270</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1222" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1222" s="6">
+        <v>44853</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1223">
+        <v>1013860</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1223" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1223" s="6">
+        <v>44880</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1224">
+        <v>988233</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1224" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1224" s="6">
+        <v>44866</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1225">
+        <v>829799</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1225" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1225" s="6">
+        <v>44876</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1226">
+        <v>338958</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1226" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1226" s="6">
+        <v>44881</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1227">
+        <v>505642</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1227" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1227" s="6">
+        <v>44874</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1228">
+        <v>862965</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1228" t="s">
+        <v>220</v>
+      </c>
+      <c r="D1228" s="6">
+        <v>44785</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1229">
+        <v>966220</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1229" s="6">
+        <v>44684</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1230">
+        <v>979924</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1230" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1230" s="6">
+        <v>44865</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1231">
+        <v>551271</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1231" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1231" s="6">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1232">
+        <v>899294</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1232" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1232" s="6">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1233">
+        <v>948276</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1233" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1233" s="6">
+        <v>44875</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1234">
+        <v>882598</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1234" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1234" s="6">
+        <v>44827</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1235">
+        <v>846778</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1235" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D1235" s="6">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1236">
+        <v>1037858</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1236" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1236" s="6">
+        <v>44874</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1237">
+        <v>872177</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1237" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1237" s="6">
+        <v>44680</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1238">
+        <v>668461</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1238" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1238" s="6">
+        <v>44874</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1239">
+        <v>1018403</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1239" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1239" s="6">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1240">
+        <v>829280</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1240" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1240" s="6">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1241">
+        <v>724495</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1241" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1241" s="6">
+        <v>44819</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>